<commit_message>
support export new translation direct to android project res value folder's strings.xml
</commit_message>
<xml_diff>
--- a/trans-sample.xlsx
+++ b/trans-sample.xlsx
@@ -19,10 +19,10 @@
     <t>key</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Chinese</t>
+    <t>values</t>
+  </si>
+  <si>
+    <t>values-zh-rCN</t>
   </si>
   <si>
     <t>civil_war</t>
@@ -66,12 +66,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +87,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
@@ -101,6 +94,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -117,6 +117,45 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,31 +169,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,32 +215,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -201,44 +224,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,6 +246,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -265,31 +402,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,139 +420,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,6 +451,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -495,15 +497,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -534,6 +527,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -548,178 +552,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,7 +1034,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1061,51 +1051,51 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimize: export to res string.xml more faster
</commit_message>
<xml_diff>
--- a/trans-sample.xlsx
+++ b/trans-sample.xlsx
@@ -19,10 +19,10 @@
     <t>key</t>
   </si>
   <si>
-    <t>values</t>
-  </si>
-  <si>
-    <t>values-zh-rCN</t>
+    <t>英语</t>
+  </si>
+  <si>
+    <t>简体中文</t>
   </si>
   <si>
     <t>civil_war</t>
@@ -66,10 +66,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -94,19 +94,27 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -116,7 +124,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,7 +140,38 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,23 +186,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,67 +230,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -246,25 +246,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +336,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,19 +348,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +366,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,97 +420,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,26 +458,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,6 +475,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,10 +522,17 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -557,148 +557,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="2"/>

</xml_diff>